<commit_message>
Atualização Casos de Uso
</commit_message>
<xml_diff>
--- a/gestao_projetos/Burndown - Sprint 1.xlsx
+++ b/gestao_projetos/Burndown - Sprint 1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1D_Gr6kfxYKhFfixTbgpEgm0NgUFvNPcI\ProjetoIntegrador\gestao_projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA4FDB5B-D1AA-4479-8F04-7BC041311844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8544E11-66B6-497D-BA2B-E6701758E951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CBD70851-FFA9-4953-93B8-5A8F85469746}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Burndown" sheetId="1" r:id="rId1"/>
+    <sheet name="Pricipais Entregas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Previsto</t>
   </si>
@@ -93,6 +94,60 @@
   </si>
   <si>
     <t>Total Horas</t>
+  </si>
+  <si>
+    <t>- Finalização das tarefas referente à prototipagem</t>
+  </si>
+  <si>
+    <t>- Criação do diagrama de classes</t>
+  </si>
+  <si>
+    <t>- Criação do diagrama de Caso  de Uso</t>
+  </si>
+  <si>
+    <t>- Ajuste do front-end do aplicativo</t>
+  </si>
+  <si>
+    <t>Principais entregas</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>qtd Horas entregues</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Observação</t>
+  </si>
+  <si>
+    <t>Pontos Positivos</t>
+  </si>
+  <si>
+    <t>Pontos Negativos</t>
+  </si>
+  <si>
+    <t>Desafios/Dificuldades</t>
+  </si>
+  <si>
+    <t>- Definir estimativa de horas coerente com cada atividade
+- Estimar o tempo útil para realização das atividades durante a sprint</t>
+  </si>
+  <si>
+    <t>- Manutenção dos status das tarefas
+- Como as demandas atravessadas são tratadas</t>
+  </si>
+  <si>
+    <t>- Auxilia na organização do que deve ser desenvolvido
+- Auxilia no planejamento do que deve ser desenvolvido</t>
+  </si>
+  <si>
+    <t>Leonardo - 00217363</t>
+  </si>
+  <si>
+    <t>Matheus - 00223804</t>
   </si>
 </sst>
 </file>
@@ -100,7 +155,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -131,15 +186,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
     </dxf>
@@ -236,7 +313,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$4</c:f>
+              <c:f>Burndown!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -271,7 +348,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$C$3:$Q$3</c:f>
+              <c:f>Burndown!$C$3:$Q$3</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -324,7 +401,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$Q$4</c:f>
+              <c:f>Burndown!$C$4:$Q$4</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
@@ -388,7 +465,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$5</c:f>
+              <c:f>Burndown!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -423,7 +500,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$C$3:$Q$3</c:f>
+              <c:f>Burndown!$C$3:$Q$3</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -476,7 +553,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$5:$Q$5</c:f>
+              <c:f>Burndown!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -502,6 +579,27 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
@@ -1272,16 +1370,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1310,7 +1408,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93DE8DFD-D1D6-45A0-AB82-B8F30C70EED0}" name="Tabela1" displayName="Tabela1" ref="B3:Q5" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93DE8DFD-D1D6-45A0-AB82-B8F30C70EED0}" name="Tabela1" displayName="Tabela1" ref="B3:Q5" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B3:Q5" xr:uid="{93DE8DFD-D1D6-45A0-AB82-B8F30C70EED0}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{EEB2BBE1-F65B-4E1B-8B42-CA7877F9CDB9}" name="Status"/>
@@ -1331,6 +1429,38 @@
     <tableColumn id="14" xr3:uid="{CE1B7677-1F36-4D37-A416-2BDF0CF4C057}" name="27/mai"/>
     <tableColumn id="15" xr3:uid="{0BED8C6D-2671-4903-A371-E28D7EEB9E94}" name="28/mai"/>
     <tableColumn id="16" xr3:uid="{3E1B9243-0953-4F04-AE25-F418D820C521}" name="29/mai"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F2C03FE8-1CF7-463B-8AF4-7A3ADEF26C12}" name="Tabela2" displayName="Tabela2" ref="S9:S13" totalsRowShown="0">
+  <autoFilter ref="S9:S13" xr:uid="{F2C03FE8-1CF7-463B-8AF4-7A3ADEF26C12}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{1A3259FF-A197-4265-9AA9-48C39EF7F840}" name="Principais entregas"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D1770603-B28B-4B36-9BBC-1140D4CD621E}" name="Tabela3" displayName="Tabela3" ref="R16:S18" totalsRowShown="0">
+  <autoFilter ref="R16:S18" xr:uid="{D1770603-B28B-4B36-9BBC-1140D4CD621E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{33C3BA2F-7FF0-4F2C-94B9-6CD31BBB2F19}" name="Equipe"/>
+    <tableColumn id="2" xr3:uid="{D0853F68-30BE-4ECD-809C-D7DCA8C5F416}" name="qtd Horas entregues" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6D2BAAC3-C224-4EBB-98A0-712B6D61083A}" name="Tabela4" displayName="Tabela4" ref="R20:S23" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="R20:S23" xr:uid="{6D2BAAC3-C224-4EBB-98A0-712B6D61083A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{98BC6D9D-7D5A-41F2-B184-091A7DDE29C1}" name="Tipo" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2A3B8B3E-BEBB-4AE6-A4F3-93B556BC6B10}" name="Observação" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1633,20 +1763,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDF5C4D-19FE-45FE-A852-02B46D48BDDE}">
-  <dimension ref="B1:Q5"/>
+  <dimension ref="B1:S23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="17" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -1654,7 +1786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -1704,7 +1836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1901,7 @@
         <v>-6.2172489379008766E-15</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1797,14 +1929,154 @@
       </c>
       <c r="J5">
         <v>16</v>
+      </c>
+      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>16</v>
+      </c>
+      <c r="O5">
+        <v>16</v>
+      </c>
+      <c r="P5">
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="R16" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R17" t="s">
+        <v>34</v>
+      </c>
+      <c r="S17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R18" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R20" t="s">
+        <v>26</v>
+      </c>
+      <c r="S20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="18:19" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="R21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="18:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="18:19" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="R23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C021128-B6EB-4D77-94DC-32749CEC7FA0}">
+  <dimension ref="B2:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 

</xml_diff>